<commit_message>
sent new version to fab, testing white soldermask
</commit_message>
<xml_diff>
--- a/PinOut.xlsx
+++ b/PinOut.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afonso Muralha\Documents\GitHub\Duckuino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\Duckuino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF922AEF-AEE0-483E-85F3-45251A5BE10F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2521A0E7-D677-4D10-86E9-0EF20667CFCE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{24732873-8C0C-4A0A-A2EE-FC5CAA2DCC25}"/>
   </bookViews>
@@ -75,12 +75,6 @@
     <t>Thumbwheel</t>
   </si>
   <si>
-    <t>Left !</t>
-  </si>
-  <si>
-    <t>Right !</t>
-  </si>
-  <si>
     <t xml:space="preserve">Center </t>
   </si>
   <si>
@@ -145,6 +139,12 @@
   </si>
   <si>
     <t>A10</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
   </si>
 </sst>
 </file>
@@ -763,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1366BAB6-4615-4638-B170-BDED74298516}">
-  <dimension ref="B1:H18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,376 +776,375 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="G9" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="4">
-        <v>2</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="4">
-        <v>3</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="15" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>